<commit_message>
Unit class has the ability to drag out stats from the csv files now...
</commit_message>
<xml_diff>
--- a/unitStats.xlsx
+++ b/unitStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moata\PycharmProjects\FantasyTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5426499-FD0F-434A-8120-4B4CAC5F87A4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CAAD62-B816-404C-9C57-35E38BB83DEB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{2FBAC523-9F6D-481A-8E54-FFF645F58D75}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" tabRatio="163" xr2:uid="{2FBAC523-9F6D-481A-8E54-FFF645F58D75}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="66">
   <si>
     <t>SPD</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>Concus</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -595,185 +598,189 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F8A5C91-975E-43D4-AEB5-A418B474C1AC}">
-  <dimension ref="A1:AC17"/>
+  <dimension ref="A1:AD17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="22.59765625" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:30" ht="15.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
       <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>57</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>53</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>55</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>54</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>53</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>55</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>54</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>53</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>19</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>53</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>39</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>13</v>
+    <row r="2" spans="1:30" ht="15.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>14</v>
-      </c>
-      <c r="C2">
-        <v>15</v>
       </c>
       <c r="D2">
         <v>15</v>
       </c>
       <c r="E2">
+        <v>15</v>
+      </c>
+      <c r="F2">
         <v>9</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>100</v>
       </c>
-      <c r="G2">
-        <v>30</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="H2">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
         <v>58</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>7</v>
       </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
       <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
         <v>25</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>95</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>20</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>15</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>20</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>21</v>
       </c>
-      <c r="Q2">
-        <v>30</v>
-      </c>
       <c r="R2">
+        <v>30</v>
+      </c>
+      <c r="S2">
         <v>90</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>1</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>22</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>45</v>
       </c>
-      <c r="V2">
-        <v>30</v>
-      </c>
       <c r="W2">
+        <v>30</v>
+      </c>
+      <c r="X2">
         <v>2</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>23</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>10</v>
       </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
       <c r="AA2">
         <v>0</v>
       </c>
@@ -781,70 +788,73 @@
         <v>0</v>
       </c>
       <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>13</v>
+    <row r="3" spans="1:30" ht="15.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="C3">
-        <v>13</v>
-      </c>
       <c r="D3">
         <v>13</v>
       </c>
       <c r="E3">
+        <v>13</v>
+      </c>
+      <c r="F3">
         <v>10</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>55</v>
       </c>
-      <c r="G3">
-        <v>30</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="H3">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s">
         <v>59</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>12</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
       <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
         <v>25</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>95</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>20</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>15</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>25</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>21</v>
       </c>
-      <c r="Q3">
-        <v>30</v>
-      </c>
       <c r="R3">
+        <v>30</v>
+      </c>
+      <c r="S3">
         <v>90</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
       <c r="U3">
         <v>0</v>
       </c>
@@ -870,88 +880,91 @@
         <v>0</v>
       </c>
       <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="1:30" ht="15.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C4">
-        <v>15</v>
       </c>
       <c r="D4">
         <v>15</v>
       </c>
       <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="F4">
         <v>9</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>100</v>
       </c>
-      <c r="G4">
-        <v>30</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="H4">
+        <v>30</v>
+      </c>
+      <c r="I4" t="s">
         <v>58</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>10</v>
       </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
       <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
         <v>25</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>95</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>20</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>25</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>35</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>21</v>
       </c>
-      <c r="Q4">
-        <v>30</v>
-      </c>
       <c r="R4">
+        <v>30</v>
+      </c>
+      <c r="S4">
         <v>90</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>1</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>22</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>45</v>
       </c>
-      <c r="V4">
-        <v>30</v>
-      </c>
       <c r="W4">
+        <v>30</v>
+      </c>
+      <c r="X4">
         <v>2</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>23</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>10</v>
       </c>
-      <c r="Z4">
-        <v>0</v>
-      </c>
       <c r="AA4">
         <v>0</v>
       </c>
@@ -959,248 +972,257 @@
         <v>0</v>
       </c>
       <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2" t="s">
+    <row r="5" spans="1:30" ht="15.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="C5">
-        <v>20</v>
       </c>
       <c r="D5">
         <v>20</v>
       </c>
       <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
         <v>9</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>100</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>35</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>58</v>
-      </c>
-      <c r="I5">
-        <v>15</v>
       </c>
       <c r="J5">
         <v>15</v>
       </c>
       <c r="K5">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="L5">
+        <v>30</v>
+      </c>
+      <c r="M5">
         <v>95</v>
       </c>
-      <c r="M5">
-        <v>30</v>
-      </c>
       <c r="N5">
+        <v>30</v>
+      </c>
+      <c r="O5">
         <v>15</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>20</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>21</v>
       </c>
-      <c r="Q5">
-        <v>30</v>
-      </c>
       <c r="R5">
+        <v>30</v>
+      </c>
+      <c r="S5">
         <v>90</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>2</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>22</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>45</v>
       </c>
-      <c r="V5">
-        <v>30</v>
-      </c>
       <c r="W5">
+        <v>30</v>
+      </c>
+      <c r="X5">
         <v>2</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>23</v>
       </c>
-      <c r="Y5">
+      <c r="Z5">
         <v>15</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>36</v>
       </c>
-      <c r="AA5">
-        <v>13</v>
-      </c>
       <c r="AB5">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="2" t="s">
+    <row r="6" spans="1:30" ht="15.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C6">
-        <v>20</v>
       </c>
       <c r="D6">
         <v>20</v>
       </c>
       <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6">
         <v>9</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>100</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>35</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>58</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>17</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>15</v>
       </c>
-      <c r="K6">
-        <v>30</v>
-      </c>
       <c r="L6">
+        <v>30</v>
+      </c>
+      <c r="M6">
         <v>95</v>
       </c>
-      <c r="M6">
-        <v>30</v>
-      </c>
       <c r="N6">
+        <v>30</v>
+      </c>
+      <c r="O6">
         <v>25</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>35</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>21</v>
       </c>
-      <c r="Q6">
-        <v>30</v>
-      </c>
       <c r="R6">
+        <v>30</v>
+      </c>
+      <c r="S6">
         <v>90</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>2</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>22</v>
       </c>
-      <c r="U6">
+      <c r="V6">
         <v>45</v>
       </c>
-      <c r="V6">
-        <v>30</v>
-      </c>
       <c r="W6">
+        <v>30</v>
+      </c>
+      <c r="X6">
         <v>2</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>23</v>
       </c>
-      <c r="Y6">
+      <c r="Z6">
         <v>15</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>38</v>
       </c>
-      <c r="AA6">
-        <v>13</v>
-      </c>
       <c r="AB6">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7">
-        <v>17</v>
+    <row r="7" spans="1:30" ht="15.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="D7">
         <v>17</v>
       </c>
       <c r="E7">
+        <v>17</v>
+      </c>
+      <c r="F7">
         <v>10</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>66</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>35</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>59</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>20</v>
       </c>
-      <c r="J7">
-        <v>13</v>
-      </c>
       <c r="K7">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="L7">
+        <v>30</v>
+      </c>
+      <c r="M7">
         <v>95</v>
       </c>
-      <c r="M7">
-        <v>30</v>
-      </c>
       <c r="N7">
+        <v>30</v>
+      </c>
+      <c r="O7">
         <v>25</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>25</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>21</v>
       </c>
-      <c r="Q7">
-        <v>30</v>
-      </c>
       <c r="R7">
+        <v>30</v>
+      </c>
+      <c r="S7">
         <v>90</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>2</v>
       </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
       <c r="U7">
         <v>0</v>
       </c>
@@ -1226,159 +1248,165 @@
         <v>0</v>
       </c>
       <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="4" t="s">
+    <row r="8" spans="1:30" ht="15.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="C8">
-        <v>25</v>
       </c>
       <c r="D8">
         <v>25</v>
       </c>
       <c r="E8">
+        <v>25</v>
+      </c>
+      <c r="F8">
         <v>9</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>100</v>
       </c>
-      <c r="G8">
-        <v>30</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="H8">
+        <v>30</v>
+      </c>
+      <c r="I8" t="s">
         <v>58</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>17</v>
       </c>
-      <c r="J8">
-        <v>30</v>
-      </c>
       <c r="K8">
         <v>30</v>
       </c>
       <c r="L8">
+        <v>30</v>
+      </c>
+      <c r="M8">
         <v>95</v>
       </c>
-      <c r="M8">
-        <v>30</v>
-      </c>
       <c r="N8">
+        <v>30</v>
+      </c>
+      <c r="O8">
         <v>25</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>35</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>21</v>
       </c>
-      <c r="Q8">
-        <v>30</v>
-      </c>
       <c r="R8">
+        <v>30</v>
+      </c>
+      <c r="S8">
         <v>90</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <v>2</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>22</v>
       </c>
-      <c r="U8">
+      <c r="V8">
         <v>45</v>
       </c>
-      <c r="V8">
-        <v>30</v>
-      </c>
       <c r="W8">
+        <v>30</v>
+      </c>
+      <c r="X8">
         <v>2</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>23</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <v>15</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AA8" t="s">
         <v>36</v>
       </c>
-      <c r="AA8">
-        <v>13</v>
-      </c>
       <c r="AB8">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="4" t="s">
+    <row r="9" spans="1:30" ht="15.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="C9">
-        <v>40</v>
       </c>
       <c r="D9">
         <v>40</v>
       </c>
       <c r="E9">
+        <v>40</v>
+      </c>
+      <c r="F9">
         <v>12</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>100</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>45</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>58</v>
       </c>
-      <c r="I9">
-        <v>30</v>
-      </c>
       <c r="J9">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="K9">
+        <v>13</v>
+      </c>
+      <c r="L9">
         <v>10</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>95</v>
       </c>
-      <c r="M9">
-        <v>30</v>
-      </c>
       <c r="N9">
-        <v>13</v>
-      </c>
-      <c r="O9" t="s">
+        <v>30</v>
+      </c>
+      <c r="O9">
+        <v>13</v>
+      </c>
+      <c r="P9" t="s">
         <v>40</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>56</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>60</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>10</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>5</v>
       </c>
-      <c r="T9">
-        <v>0</v>
-      </c>
       <c r="U9">
         <v>0</v>
       </c>
@@ -1388,430 +1416,445 @@
       <c r="W9">
         <v>0</v>
       </c>
-      <c r="X9" t="s">
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9" t="s">
         <v>47</v>
       </c>
-      <c r="Y9">
+      <c r="Z9">
         <v>45</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="AA9" t="s">
         <v>48</v>
       </c>
-      <c r="AA9">
+      <c r="AB9">
         <v>50</v>
       </c>
-      <c r="AB9">
-        <v>0</v>
-      </c>
       <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="4" t="s">
+    <row r="10" spans="1:30" ht="15.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>55</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>5</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>12</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>100</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>45</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>58</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>37</v>
       </c>
-      <c r="J10">
-        <v>13</v>
-      </c>
       <c r="K10">
+        <v>13</v>
+      </c>
+      <c r="L10">
         <v>10</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>95</v>
       </c>
-      <c r="M10">
-        <v>30</v>
-      </c>
       <c r="N10">
-        <v>13</v>
-      </c>
-      <c r="O10" t="s">
+        <v>30</v>
+      </c>
+      <c r="O10">
+        <v>13</v>
+      </c>
+      <c r="P10" t="s">
         <v>35</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>56</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>80</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>10</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <v>5</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
         <v>22</v>
       </c>
-      <c r="U10">
+      <c r="V10">
         <v>45</v>
       </c>
-      <c r="V10">
-        <v>30</v>
-      </c>
       <c r="W10">
+        <v>30</v>
+      </c>
+      <c r="X10">
         <v>2</v>
       </c>
-      <c r="X10">
-        <v>0</v>
-      </c>
       <c r="Y10">
         <v>0</v>
       </c>
-      <c r="Z10" t="s">
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10" t="s">
         <v>48</v>
       </c>
-      <c r="AA10">
-        <v>13</v>
-      </c>
-      <c r="AB10" t="s">
+      <c r="AB10">
+        <v>13</v>
+      </c>
+      <c r="AC10" t="s">
         <v>46</v>
       </c>
-      <c r="AC10">
+      <c r="AD10">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="4" t="s">
+    <row r="11" spans="1:30" ht="15.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="C11">
-        <v>23</v>
       </c>
       <c r="D11">
         <v>23</v>
       </c>
       <c r="E11">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F11">
+        <v>13</v>
+      </c>
+      <c r="G11">
         <v>200</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>100</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>58</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>40</v>
       </c>
-      <c r="J11">
-        <v>13</v>
-      </c>
       <c r="K11">
+        <v>13</v>
+      </c>
+      <c r="L11">
         <v>70</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>95</v>
       </c>
-      <c r="M11">
-        <v>13</v>
-      </c>
       <c r="N11">
         <v>13</v>
       </c>
-      <c r="O11" t="s">
+      <c r="O11">
+        <v>13</v>
+      </c>
+      <c r="P11" t="s">
         <v>35</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>21</v>
       </c>
-      <c r="Q11">
-        <v>30</v>
-      </c>
       <c r="R11">
+        <v>30</v>
+      </c>
+      <c r="S11">
         <v>90</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <v>2</v>
       </c>
-      <c r="T11" t="s">
+      <c r="U11" t="s">
         <v>43</v>
       </c>
-      <c r="U11">
+      <c r="V11">
         <v>95</v>
       </c>
-      <c r="V11">
+      <c r="W11">
         <v>10</v>
       </c>
-      <c r="W11">
+      <c r="X11">
         <v>4</v>
       </c>
-      <c r="X11" t="s">
+      <c r="Y11" t="s">
         <v>44</v>
       </c>
-      <c r="Y11">
+      <c r="Z11">
         <v>55</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="AA11" t="s">
         <v>45</v>
       </c>
-      <c r="AA11">
+      <c r="AB11">
         <v>17</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AC11" t="s">
         <v>42</v>
       </c>
-      <c r="AC11">
+      <c r="AD11">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="4" t="s">
+    <row r="12" spans="1:30" ht="15.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="C12">
-        <v>37</v>
       </c>
       <c r="D12">
         <v>37</v>
       </c>
       <c r="E12">
+        <v>37</v>
+      </c>
+      <c r="F12">
         <v>9</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>100</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>27</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>58</v>
       </c>
-      <c r="I12">
-        <v>30</v>
-      </c>
       <c r="J12">
+        <v>30</v>
+      </c>
+      <c r="K12">
         <v>36</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>35</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>95</v>
-      </c>
-      <c r="M12">
-        <v>80</v>
       </c>
       <c r="N12">
         <v>80</v>
       </c>
-      <c r="O12" t="s">
+      <c r="O12">
+        <v>80</v>
+      </c>
+      <c r="P12" t="s">
         <v>20</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>21</v>
       </c>
-      <c r="Q12">
-        <v>30</v>
-      </c>
       <c r="R12">
+        <v>30</v>
+      </c>
+      <c r="S12">
         <v>90</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <v>2</v>
       </c>
-      <c r="T12" t="s">
+      <c r="U12" t="s">
         <v>22</v>
       </c>
-      <c r="U12">
+      <c r="V12">
         <v>45</v>
       </c>
-      <c r="V12">
-        <v>30</v>
-      </c>
       <c r="W12">
+        <v>30</v>
+      </c>
+      <c r="X12">
         <v>2</v>
       </c>
-      <c r="X12" t="s">
+      <c r="Y12" t="s">
         <v>44</v>
       </c>
-      <c r="Y12">
+      <c r="Z12">
         <v>55</v>
       </c>
-      <c r="Z12" t="s">
+      <c r="AA12" t="s">
         <v>45</v>
       </c>
-      <c r="AA12">
+      <c r="AB12">
         <v>17</v>
       </c>
-      <c r="AB12">
-        <v>0</v>
-      </c>
       <c r="AC12">
+        <v>0</v>
+      </c>
+      <c r="AD12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13">
+    <row r="13" spans="1:30" ht="15.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D13">
         <v>37</v>
       </c>
       <c r="E13">
+        <v>37</v>
+      </c>
+      <c r="F13">
         <v>9</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>100</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>27</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>58</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>37</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>36</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>35</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>95</v>
-      </c>
-      <c r="M13">
-        <v>80</v>
       </c>
       <c r="N13">
         <v>80</v>
       </c>
-      <c r="O13" t="s">
+      <c r="O13">
+        <v>80</v>
+      </c>
+      <c r="P13" t="s">
         <v>35</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>21</v>
       </c>
-      <c r="Q13">
-        <v>30</v>
-      </c>
       <c r="R13">
+        <v>30</v>
+      </c>
+      <c r="S13">
         <v>90</v>
       </c>
-      <c r="S13">
+      <c r="T13">
         <v>2</v>
       </c>
-      <c r="T13" t="s">
+      <c r="U13" t="s">
         <v>22</v>
       </c>
-      <c r="U13">
+      <c r="V13">
         <v>45</v>
       </c>
-      <c r="V13">
-        <v>30</v>
-      </c>
       <c r="W13">
+        <v>30</v>
+      </c>
+      <c r="X13">
         <v>2</v>
       </c>
-      <c r="X13" t="s">
+      <c r="Y13" t="s">
         <v>44</v>
       </c>
-      <c r="Y13">
+      <c r="Z13">
         <v>55</v>
       </c>
-      <c r="Z13" t="s">
+      <c r="AA13" t="s">
         <v>45</v>
       </c>
-      <c r="AA13">
+      <c r="AB13">
         <v>17</v>
       </c>
-      <c r="AB13">
-        <v>0</v>
-      </c>
       <c r="AC13">
+        <v>0</v>
+      </c>
+      <c r="AD13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="4" t="s">
+    <row r="14" spans="1:30" ht="15.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="C14">
-        <v>15</v>
       </c>
       <c r="D14">
         <v>15</v>
       </c>
       <c r="E14">
+        <v>15</v>
+      </c>
+      <c r="F14">
         <v>3</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>70</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>27</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>59</v>
       </c>
-      <c r="I14">
-        <v>30</v>
-      </c>
       <c r="J14">
+        <v>30</v>
+      </c>
+      <c r="K14">
         <v>40</v>
       </c>
-      <c r="K14">
-        <v>30</v>
-      </c>
       <c r="L14">
+        <v>30</v>
+      </c>
+      <c r="M14">
         <v>95</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>15</v>
       </c>
-      <c r="N14">
-        <v>30</v>
-      </c>
-      <c r="O14" t="s">
+      <c r="O14">
+        <v>30</v>
+      </c>
+      <c r="P14" t="s">
         <v>60</v>
       </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
       <c r="Q14">
         <v>0</v>
       </c>
@@ -1849,70 +1892,73 @@
         <v>0</v>
       </c>
       <c r="AC14">
+        <v>0</v>
+      </c>
+      <c r="AD14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="4" t="s">
+    <row r="15" spans="1:30" ht="15.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C15">
-        <v>30</v>
-      </c>
       <c r="D15">
         <v>30</v>
       </c>
       <c r="E15">
+        <v>30</v>
+      </c>
+      <c r="F15">
         <v>7</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>80</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>27</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>59</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>35</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>40</v>
       </c>
-      <c r="K15">
-        <v>30</v>
-      </c>
       <c r="L15">
+        <v>30</v>
+      </c>
+      <c r="M15">
         <v>95</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>15</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>50</v>
       </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15" t="s">
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="s">
         <v>60</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>90</v>
       </c>
-      <c r="R15">
+      <c r="S15">
         <v>50</v>
       </c>
-      <c r="S15">
+      <c r="T15">
         <v>5</v>
       </c>
-      <c r="T15">
-        <v>0</v>
-      </c>
       <c r="U15">
         <v>0</v>
       </c>
@@ -1938,58 +1984,61 @@
         <v>0</v>
       </c>
       <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AD15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="4" t="s">
+    <row r="16" spans="1:30" ht="15.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>20</v>
       </c>
-      <c r="D16">
-        <v>13</v>
-      </c>
       <c r="E16">
+        <v>13</v>
+      </c>
+      <c r="F16">
         <v>9</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>100</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>27</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>58</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>7</v>
       </c>
-      <c r="J16">
-        <v>30</v>
-      </c>
       <c r="K16">
         <v>30</v>
       </c>
       <c r="L16">
+        <v>30</v>
+      </c>
+      <c r="M16">
         <v>95</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>15</v>
       </c>
-      <c r="N16">
-        <v>13</v>
-      </c>
-      <c r="O16" t="s">
+      <c r="O16">
+        <v>13</v>
+      </c>
+      <c r="P16" t="s">
         <v>20</v>
       </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
       <c r="Q16">
         <v>0</v>
       </c>
@@ -2023,62 +2072,65 @@
       <c r="AA16">
         <v>0</v>
       </c>
-      <c r="AB16" t="s">
+      <c r="AB16">
+        <v>0</v>
+      </c>
+      <c r="AC16" t="s">
         <v>61</v>
       </c>
-      <c r="AC16">
+      <c r="AD16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="4" t="s">
+    <row r="17" spans="1:30" ht="15.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="C17">
-        <v>80</v>
       </c>
       <c r="D17">
         <v>80</v>
       </c>
       <c r="E17">
+        <v>80</v>
+      </c>
+      <c r="F17">
         <v>10</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>100</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>50</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>58</v>
-      </c>
-      <c r="I17">
-        <v>50</v>
       </c>
       <c r="J17">
         <v>50</v>
       </c>
       <c r="K17">
+        <v>50</v>
+      </c>
+      <c r="L17">
         <v>40</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>105</v>
-      </c>
-      <c r="M17">
-        <v>100</v>
       </c>
       <c r="N17">
         <v>100</v>
       </c>
-      <c r="O17" t="s">
+      <c r="O17">
+        <v>100</v>
+      </c>
+      <c r="P17" t="s">
         <v>62</v>
       </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
       <c r="Q17">
         <v>0</v>
       </c>
@@ -2100,22 +2152,25 @@
       <c r="W17">
         <v>0</v>
       </c>
-      <c r="X17" t="s">
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17" t="s">
         <v>63</v>
       </c>
-      <c r="Y17">
+      <c r="Z17">
         <v>80</v>
       </c>
-      <c r="Z17" t="s">
+      <c r="AA17" t="s">
         <v>64</v>
       </c>
-      <c r="AA17">
+      <c r="AB17">
         <v>75</v>
       </c>
-      <c r="AB17">
-        <v>0</v>
-      </c>
       <c r="AC17">
+        <v>0</v>
+      </c>
+      <c r="AD17">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
NPC Class started, atrributes are finished I'm prety sure, also if self.*insertstathere* is done for parent class too
</commit_message>
<xml_diff>
--- a/unitStats.xlsx
+++ b/unitStats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moata\PycharmProjects\FantasyTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CAAD62-B816-404C-9C57-35E38BB83DEB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EE0799-BD6D-47B5-BF0E-BDC44B4894D5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" tabRatio="163" xr2:uid="{2FBAC523-9F6D-481A-8E54-FFF645F58D75}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="69">
   <si>
     <t>SPD</t>
   </si>
@@ -192,9 +192,6 @@
     <t>RatOgre</t>
   </si>
   <si>
-    <t>%</t>
-  </si>
-  <si>
     <t>DOT</t>
   </si>
   <si>
@@ -229,6 +226,18 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>Blight%Chance</t>
+  </si>
+  <si>
+    <t>Bleed%Chance</t>
+  </si>
+  <si>
+    <t>Move%Chance</t>
+  </si>
+  <si>
+    <t>Stun%Chance</t>
   </si>
 </sst>
 </file>
@@ -601,7 +610,7 @@
   <dimension ref="A1:AD17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -612,7 +621,7 @@
   <sheetData>
     <row r="1" spans="1:30" ht="15.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -636,7 +645,7 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J1" t="s">
         <v>8</v>
@@ -663,37 +672,37 @@
         <v>16</v>
       </c>
       <c r="R1" t="s">
+        <v>65</v>
+      </c>
+      <c r="S1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T1" t="s">
         <v>53</v>
-      </c>
-      <c r="S1" t="s">
-        <v>55</v>
-      </c>
-      <c r="T1" t="s">
-        <v>54</v>
       </c>
       <c r="U1" t="s">
         <v>17</v>
       </c>
       <c r="V1" t="s">
+        <v>66</v>
+      </c>
+      <c r="W1" t="s">
+        <v>54</v>
+      </c>
+      <c r="X1" t="s">
         <v>53</v>
-      </c>
-      <c r="W1" t="s">
-        <v>55</v>
-      </c>
-      <c r="X1" t="s">
-        <v>54</v>
       </c>
       <c r="Y1" t="s">
         <v>18</v>
       </c>
       <c r="Z1" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="AA1" t="s">
         <v>19</v>
       </c>
       <c r="AB1" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="AC1" t="s">
         <v>39</v>
@@ -728,7 +737,7 @@
         <v>30</v>
       </c>
       <c r="I2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J2">
         <v>7</v>
@@ -820,7 +829,7 @@
         <v>30</v>
       </c>
       <c r="I3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J3">
         <v>12</v>
@@ -912,7 +921,7 @@
         <v>30</v>
       </c>
       <c r="I4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J4">
         <v>10</v>
@@ -1004,7 +1013,7 @@
         <v>35</v>
       </c>
       <c r="I5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J5">
         <v>15</v>
@@ -1096,7 +1105,7 @@
         <v>35</v>
       </c>
       <c r="I6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J6">
         <v>17</v>
@@ -1188,7 +1197,7 @@
         <v>35</v>
       </c>
       <c r="I7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J7">
         <v>20</v>
@@ -1280,7 +1289,7 @@
         <v>30</v>
       </c>
       <c r="I8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J8">
         <v>17</v>
@@ -1372,7 +1381,7 @@
         <v>45</v>
       </c>
       <c r="I9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J9">
         <v>30</v>
@@ -1396,7 +1405,7 @@
         <v>40</v>
       </c>
       <c r="Q9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R9">
         <v>60</v>
@@ -1464,7 +1473,7 @@
         <v>45</v>
       </c>
       <c r="I10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J10">
         <v>37</v>
@@ -1488,7 +1497,7 @@
         <v>35</v>
       </c>
       <c r="Q10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R10">
         <v>80</v>
@@ -1556,7 +1565,7 @@
         <v>100</v>
       </c>
       <c r="I11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J11">
         <v>40</v>
@@ -1648,7 +1657,7 @@
         <v>27</v>
       </c>
       <c r="I12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J12">
         <v>30</v>
@@ -1740,7 +1749,7 @@
         <v>27</v>
       </c>
       <c r="I13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J13">
         <v>37</v>
@@ -1832,7 +1841,7 @@
         <v>27</v>
       </c>
       <c r="I14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J14">
         <v>30</v>
@@ -1853,7 +1862,7 @@
         <v>30</v>
       </c>
       <c r="P14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q14">
         <v>0</v>
@@ -1924,7 +1933,7 @@
         <v>27</v>
       </c>
       <c r="I15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J15">
         <v>35</v>
@@ -1948,7 +1957,7 @@
         <v>0</v>
       </c>
       <c r="Q15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R15">
         <v>90</v>
@@ -2016,7 +2025,7 @@
         <v>27</v>
       </c>
       <c r="I16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J16">
         <v>7</v>
@@ -2076,7 +2085,7 @@
         <v>0</v>
       </c>
       <c r="AC16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AD16">
         <v>1</v>
@@ -2108,7 +2117,7 @@
         <v>50</v>
       </c>
       <c r="I17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J17">
         <v>50</v>
@@ -2129,40 +2138,40 @@
         <v>100</v>
       </c>
       <c r="P17" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17" t="s">
         <v>62</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-      <c r="R17">
-        <v>0</v>
-      </c>
-      <c r="S17">
-        <v>0</v>
-      </c>
-      <c r="T17">
-        <v>0</v>
-      </c>
-      <c r="U17">
-        <v>0</v>
-      </c>
-      <c r="V17">
-        <v>0</v>
-      </c>
-      <c r="W17">
-        <v>0</v>
-      </c>
-      <c r="X17">
-        <v>0</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>63</v>
       </c>
       <c r="Z17">
         <v>80</v>
       </c>
       <c r="AA17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AB17">
         <v>75</v>

</xml_diff>